<commit_message>
Ajustes lancamentos e titulos VGV
</commit_message>
<xml_diff>
--- a/Relatorio_Completo_Residencial_2025_11.xlsx
+++ b/Relatorio_Completo_Residencial_2025_11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandregarcia/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284CC6A2-35DC-8E42-87CC-CACCB6B90CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBA1A43-97DB-204B-AFFC-45C81F0587CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" firstSheet="34" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <t>Gerado em:</t>
   </si>
   <si>
-    <t>25/12/2025, 10:56:47</t>
+    <t>07/01/2026, 15:42:51</t>
   </si>
   <si>
     <t>Filtros e configurações aplicadas:</t>
@@ -843,7 +843,7 @@
     <t>418 [2]</t>
   </si>
   <si>
-    <t>496 [0]</t>
+    <t>496 [1]</t>
   </si>
   <si>
     <t>105 [1]</t>
@@ -891,7 +891,7 @@
     <t>852 [6]</t>
   </si>
   <si>
-    <t>732 [2]</t>
+    <t>732 [3]</t>
   </si>
   <si>
     <t>1.029 [5]</t>
@@ -1002,7 +1002,7 @@
     <t>667 [6]</t>
   </si>
   <si>
-    <t>526 [1]</t>
+    <t>526 [2]</t>
   </si>
   <si>
     <t>177 [2]</t>
@@ -1011,7 +1011,7 @@
     <t>1.146 [10]</t>
   </si>
   <si>
-    <t>1.072 [8]</t>
+    <t>1.072 [9]</t>
   </si>
   <si>
     <t>1.986 [10]</t>
@@ -1059,7 +1059,7 @@
     <t>4.861 [40]</t>
   </si>
   <si>
-    <t>3.271 [23]</t>
+    <t>3.271 [24]</t>
   </si>
   <si>
     <t>-32,7%</t>
@@ -1071,7 +1071,7 @@
     <t>+77,6%</t>
   </si>
   <si>
-    <t>2.353 [18]</t>
+    <t>2.353 [19]</t>
   </si>
   <si>
     <t>-59,5%</t>
@@ -4237,7 +4237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6099,10 +6099,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4379604-D300-0748-86EA-4F998E872AC9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6552F771-1FF9-0E47-9891-261ADFAC565B}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -8189,7 +8189,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EC704-CC5A-2B44-8E09-245412CEF2AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3011B6-10B6-5B45-9E44-C757FCC3FFFF}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10221,7 +10221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559E24AA-559D-7F47-A6E9-D6AE892D2F29}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE0F23A-13AB-8344-AC5E-92451A96D224}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11159,7 +11159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C055B75C-AB4B-A948-B191-DB5B24382D75}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3D112A-008F-CA43-8E41-15EEA5BF07B4}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11583,7 +11583,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A018EAC7-D32F-FB43-8F86-340EC1E7E0A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E8F359-FE85-B444-BCB0-DCC7015646AE}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>